<commit_message>
need to improve the method printBill to create the kgTable ..
so far so good
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice/invoice.xlsx
+++ b/src/main/resources/invoice/invoice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Software Solutions\trial 1\src\main\resources\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0849131A-8D0B-4133-A93C-A5C72BEA3902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D5255E-F7F5-429B-B20B-A5C2AC70CEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>සැපයුම් කරුගේ නම</t>
   </si>
@@ -75,15 +75,9 @@
     <t>වෙනත්</t>
   </si>
   <si>
-    <t xml:space="preserve">මුද්දර </t>
-  </si>
-  <si>
     <t>ඉතිරි මුදල</t>
   </si>
   <si>
-    <t>ඉදිරියට ගෙන ආ කාසි</t>
-  </si>
-  <si>
     <t xml:space="preserve">ගෙවන  මුදල </t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>කිලෝ ග්‍රෑම්</t>
   </si>
   <si>
-    <t>බිල් අංකය 231001</t>
-  </si>
-  <si>
     <t xml:space="preserve">           KAPILA TEA FACTORY</t>
   </si>
   <si>
@@ -202,6 +193,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 070-4564645</t>
+  </si>
+  <si>
+    <t>මුළු වියදම් එකතුව</t>
+  </si>
+  <si>
+    <t>බිල් අංකය 0000</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,27 +378,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -409,6 +412,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,13 +540,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -585,13 +591,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1047750</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -636,13 +642,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -948,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,20 +975,20 @@
     <col min="11" max="11" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>57</v>
+    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+        <v>55</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -995,11 +1001,11 @@
       <c r="B2" s="2">
         <v>1196</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1013,18 +1019,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="23"/>
+      <c r="D3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="I3" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1043,7 +1049,7 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="12">
         <f>SUM(E8:E16) + SUM(G8:G16) + SUM(I8:I16) + SUM(K8:K16)</f>
         <v>26</v>
       </c>
@@ -1054,11 +1060,11 @@
         <v>5</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1077,270 +1083,264 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="6">
+      <c r="C7" s="17">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>21</v>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="6">
+      <c r="C8" s="17">
         <v>3990</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="D8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13">
         <v>2</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="18"/>
+      <c r="F8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="6">
+      <c r="C9" s="17">
         <v>0</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="13">
         <v>3</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="16">
+      <c r="F9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="13">
         <v>2</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="16">
+      <c r="H9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="13">
         <v>5</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="18">
+      <c r="J9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f>SUM(C7:C9)</f>
         <v>4000</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="18"/>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
+        <v>105</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="13">
+        <v>12</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="18">
+        <v>100</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="13" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="13" t="s">
+      <c r="G14" s="13"/>
+      <c r="H14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="18"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="11">
-        <v>105</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="13" t="s">
+      <c r="I14" s="13"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="16">
-        <v>12</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="13" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="18"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="11">
-        <v>100</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="13" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="13" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="13" t="s">
+      <c r="G16" s="14"/>
+      <c r="H16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11">
+      <c r="I16" s="14"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="18">
         <v>0</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="11">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="11">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="11">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1351,28 +1351,30 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="11">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="5">
+        <f>SUM(C12:C17)</f>
+        <v>205</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="14"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="6">
-        <f>SUM(B12:B18)</f>
-        <v>205</v>
+      <c r="C19" s="5">
+        <v>0</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1383,30 +1385,15 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="6">
-        <f>SUM(C10+C19)</f>
-        <v>4205</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="9">
+        <f>SUM(C19)</f>
+        <v>0</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1417,13 +1404,9 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="12">
-        <v>4205</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1485,40 +1468,15 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="I3:K3"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.25" right="0.05" top="0" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
creation of xlsx are done whats left is that to implement the method printSelectedBills
what need to be done is that send the created xlsx file to the printer to printer without that sheet at the index 0;
</commit_message>
<xml_diff>
--- a/src/main/resources/invoice/invoice.xlsx
+++ b/src/main/resources/invoice/invoice.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Software Solutions\trial 1\src\main\resources\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D5255E-F7F5-429B-B20B-A5C2AC70CEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EF7717-2D28-4EA5-BA1E-5DD400BDA24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="1275" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$21</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -205,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +261,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei UI Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -400,20 +409,19 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,13 +990,13 @@
       <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1001,11 +1009,11 @@
       <c r="B2" s="2">
         <v>1196</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1019,18 +1027,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1060,11 +1068,11 @@
         <v>5</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1082,12 +1090,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="17">
+      <c r="C7" s="19">
         <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1115,12 +1123,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="17">
+      <c r="C8" s="19">
         <v>3990</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1142,12 +1150,12 @@
       </c>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="17">
+      <c r="C9" s="19">
         <v>0</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -1176,7 +1184,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
@@ -1223,10 +1231,10 @@
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>105</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -1247,10 +1255,10 @@
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>100</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1269,10 +1277,10 @@
       <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>0</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1291,10 +1299,10 @@
       <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1313,10 +1321,10 @@
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="17">
         <v>0</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -1335,10 +1343,10 @@
       <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <v>0</v>
       </c>
       <c r="D17" s="1"/>
@@ -1476,8 +1484,8 @@
     <mergeCell ref="F5:H5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.1" right="0" top="0.75" bottom="0" header="0.3" footer="0"/>
+  <pageSetup paperSize="11" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>